<commit_message>
mejora de consulta - HospitalLocator
</commit_message>
<xml_diff>
--- a/Python_hacks/Hospitales/hospitales_geocodificados.xlsx
+++ b/Python_hacks/Hospitales/hospitales_geocodificados.xlsx
@@ -10444,7 +10444,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -10508,16 +10508,16 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -10838,7 +10838,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="31.433571428571426" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -10865,7 +10865,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4">
         <v>8734</v>
       </c>
@@ -10885,7 +10885,7 @@
         <v>-99.0688279</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4">
         <v>10316</v>
       </c>
@@ -10905,7 +10905,7 @@
         <v>-98.100684</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4">
         <v>10317</v>
       </c>
@@ -10925,7 +10925,7 @@
         <v>-97.3489729</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4">
         <v>10319</v>
       </c>
@@ -10945,7 +10945,7 @@
         <v>-97.5232604</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4">
         <v>7733</v>
       </c>
@@ -10961,7 +10961,7 @@
         <v>-115.0937357</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4">
         <v>7734</v>
       </c>
@@ -10977,7 +10977,7 @@
         <v>-115.1394211</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4">
         <v>7735</v>
       </c>
@@ -10993,7 +10993,7 @@
         <v>-102.1943485</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4">
         <v>7736</v>
       </c>
@@ -11009,7 +11009,7 @@
         <v>-117.0559787</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4">
         <v>7738</v>
       </c>
@@ -11025,7 +11025,7 @@
         <v>-115.4186163</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4">
         <v>7739</v>
       </c>
@@ -11041,7 +11041,7 @@
         <v>-115.495201</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4">
         <v>7740</v>
       </c>
@@ -11057,7 +11057,7 @@
         <v>-115.4565988</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4">
         <v>7741</v>
       </c>
@@ -11073,7 +11073,7 @@
         <v>-102.552784</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4">
         <v>7742</v>
       </c>
@@ -11089,7 +11089,7 @@
         <v>-100.5317209</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4">
         <v>7743</v>
       </c>
@@ -11105,7 +11105,7 @@
         <v>-115.1013143</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4">
         <v>7744</v>
       </c>
@@ -11121,7 +11121,7 @@
         <v>-116.8317806</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4">
         <v>7745</v>
       </c>
@@ -11137,7 +11137,7 @@
         <v>-104.6608131</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="4">
         <v>7746</v>
       </c>
@@ -11153,7 +11153,7 @@
         <v>-116.9021914</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="4">
         <v>7748</v>
       </c>
@@ -11169,7 +11169,7 @@
         <v>-116.6312331</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4">
         <v>7749</v>
       </c>
@@ -11185,7 +11185,7 @@
         <v>-116.5920782</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4">
         <v>7750</v>
       </c>
@@ -11201,7 +11201,7 @@
         <v>-116.696322</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="4">
         <v>7751</v>
       </c>
@@ -11217,7 +11217,7 @@
         <v>-116.9402112</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="4">
         <v>7752</v>
       </c>
@@ -11233,7 +11233,7 @@
         <v>-117.0448389</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="4">
         <v>7753</v>
       </c>
@@ -11249,7 +11249,7 @@
         <v>-117.075746</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="4">
         <v>7754</v>
       </c>
@@ -11265,7 +11265,7 @@
         <v>-110.9559192</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="4">
         <v>7755</v>
       </c>
@@ -11281,7 +11281,7 @@
         <v>-99.1013498</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="4">
         <v>7756</v>
       </c>
@@ -11297,7 +11297,7 @@
         <v>-99.1591014</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="4">
         <v>7757</v>
       </c>
@@ -11313,7 +11313,7 @@
         <v>-99.99619469999999</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="4">
         <v>7758</v>
       </c>

</xml_diff>